<commit_message>
Melborne city page import pending
</commit_message>
<xml_diff>
--- a/src/ExcelSheetIO/BigIssueRostering.xlsx
+++ b/src/ExcelSheetIO/BigIssueRostering.xlsx
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1689" uniqueCount="174">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1690" uniqueCount="175">
   <si>
     <t>Day</t>
   </si>
@@ -562,6 +562,9 @@
   <si>
     <t>No</t>
   </si>
+  <si>
+    <t>ddddddd</t>
+  </si>
 </sst>
 </file>
 
@@ -570,13 +573,12 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
   </numFmts>
-  <fonts count="16" x14ac:knownFonts="1">
+  <fonts count="17" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <charset val="136"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -684,6 +686,14 @@
     <font>
       <sz val="12"/>
       <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -913,13 +923,14 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="6">
+  <cellStyleXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="41">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -994,8 +1005,9 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="6">
+  <cellStyles count="7">
     <cellStyle name="Calculation" xfId="2" builtinId="22"/>
+    <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8"/>
     <cellStyle name="Input" xfId="1" builtinId="20"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -8358,10 +8370,10 @@
   <dimension ref="A1:AH43"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" view="pageBreakPreview" zoomScale="92" zoomScaleSheetLayoutView="50" workbookViewId="0">
-      <pane xSplit="3" ySplit="1" topLeftCell="F2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="1" topLeftCell="U2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="H2" sqref="H2"/>
+      <selection pane="bottomRight" activeCell="V11" sqref="V11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -8506,10 +8518,10 @@
         <v>173</v>
       </c>
       <c r="I2" s="12">
-        <v>0.45833333333333331</v>
+        <v>0.66666666666666663</v>
       </c>
       <c r="J2" s="12">
-        <v>0.52083333333333337</v>
+        <v>0.70833333333333337</v>
       </c>
       <c r="K2" s="12"/>
       <c r="L2" s="12"/>
@@ -8535,8 +8547,12 @@
       <c r="T2" s="3"/>
       <c r="U2" s="3"/>
       <c r="V2" s="3"/>
-      <c r="W2" s="3"/>
-      <c r="X2" s="3"/>
+      <c r="W2" s="12">
+        <v>0.6875</v>
+      </c>
+      <c r="X2" s="3" t="s">
+        <v>174</v>
+      </c>
       <c r="Y2" s="3"/>
       <c r="Z2" s="3"/>
       <c r="AA2" s="3"/>
@@ -10214,7 +10230,7 @@
     </row>
   </sheetData>
   <dataValidations count="5">
-    <dataValidation type="time" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="L2 I2:K3 M2:P3 R2:V43 I4:P43">
+    <dataValidation type="time" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="L2 I2:K3 M2:P3 R2:V43 I4:P43 W2">
       <formula1>0.375</formula1>
       <formula2>0.708333333333333</formula2>
     </dataValidation>
@@ -10233,6 +10249,7 @@
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>

<commit_message>
Changes to the pairTeams method plus adding of new method to optimize team selection
</commit_message>
<xml_diff>
--- a/src/ExcelSheetIO/BigIssueRostering.xlsx
+++ b/src/ExcelSheetIO/BigIssueRostering.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Joao/Documents/GitHub/swen90014-2019-bi-bilby/src/ExcelSheetIO/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C6AD572-C805-194D-9214-AD60D8CDB20F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF17027E-BF8C-7B40-AE50-6FB7F1162A1D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="33600" windowHeight="21000" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="20540" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Summary - Cities" sheetId="7" r:id="rId1"/>
@@ -518,9 +518,6 @@
     <t>Yes</t>
   </si>
   <si>
-    <t>No</t>
-  </si>
-  <si>
     <t xml:space="preserve">Workshop </t>
   </si>
   <si>
@@ -546,9 +543,6 @@
   </si>
   <si>
     <t>P123,DHD,HHIe</t>
-  </si>
-  <si>
-    <t>P123,DHD,HHIe,C</t>
   </si>
   <si>
     <t>Specific Unavailability 1 From</t>
@@ -617,7 +611,13 @@
     <t>P123,P456,DHD,HHIe</t>
   </si>
   <si>
-    <t>P123,DHD,HHIe,TBIdea</t>
+    <t>P123,DHD,TBIdea,HHIe</t>
+  </si>
+  <si>
+    <t>P123,DHD,C,HHIe</t>
+  </si>
+  <si>
+    <t>P123,DHD,TBIdea,C,HHIe</t>
   </si>
 </sst>
 </file>
@@ -790,7 +790,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="16">
+  <borders count="18">
     <border>
       <left/>
       <right/>
@@ -997,6 +997,32 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="hair">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="hair">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="hair">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -1009,7 +1035,7 @@
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="46">
+  <cellXfs count="51">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -1058,6 +1084,11 @@
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="14" fontId="1" fillId="2" borderId="1" xfId="1" applyNumberFormat="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="20" fontId="15" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="20" fontId="15" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="20" fontId="0" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1"/>
+    <xf numFmtId="20" fontId="15" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="9" xfId="4" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1211,7 +1242,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light"/>
+        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -1263,7 +1294,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -3960,10 +3991,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="B1" s="36" t="s">
+      <c r="B1" s="41" t="s">
         <v>3</v>
       </c>
-      <c r="C1" s="36"/>
+      <c r="C1" s="41"/>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.2">
       <c r="B2" s="16" t="s">
@@ -6610,16 +6641,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A1" s="37" t="s">
+      <c r="A1" s="42" t="s">
         <v>2</v>
       </c>
-      <c r="B1" s="37"/>
-      <c r="C1" s="37"/>
-      <c r="E1" s="38" t="s">
+      <c r="B1" s="42"/>
+      <c r="C1" s="42"/>
+      <c r="E1" s="43" t="s">
         <v>9</v>
       </c>
-      <c r="F1" s="39"/>
-      <c r="G1" s="39"/>
+      <c r="F1" s="44"/>
+      <c r="G1" s="44"/>
     </row>
     <row r="2" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A2" s="23" t="s">
@@ -6633,13 +6664,13 @@
       </c>
       <c r="D2" s="18"/>
       <c r="E2" s="23" t="s">
+        <v>157</v>
+      </c>
+      <c r="F2" s="23" t="s">
         <v>158</v>
       </c>
-      <c r="F2" s="23" t="s">
+      <c r="G2" s="23" t="s">
         <v>159</v>
-      </c>
-      <c r="G2" s="23" t="s">
-        <v>160</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.2">
@@ -6979,13 +7010,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A1" s="40" t="s">
+      <c r="A1" s="45" t="s">
         <v>60</v>
       </c>
-      <c r="B1" s="41"/>
-      <c r="C1" s="41"/>
-      <c r="D1" s="41"/>
-      <c r="E1" s="41"/>
+      <c r="B1" s="46"/>
+      <c r="C1" s="46"/>
+      <c r="D1" s="46"/>
+      <c r="E1" s="46"/>
     </row>
     <row r="2" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A2" s="23" t="s">
@@ -8227,10 +8258,10 @@
   <dimension ref="A1:AN43"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" view="pageBreakPreview" zoomScale="92" zoomScaleSheetLayoutView="50" workbookViewId="0">
-      <pane xSplit="3" ySplit="1" topLeftCell="D2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="1" topLeftCell="F2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="H20" sqref="H20"/>
+      <selection pane="bottomRight" activeCell="K20" sqref="K20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -8327,58 +8358,58 @@
         <v>74</v>
       </c>
       <c r="W1" s="23" t="s">
+        <v>166</v>
+      </c>
+      <c r="X1" s="23" t="s">
+        <v>167</v>
+      </c>
+      <c r="Y1" s="23" t="s">
+        <v>178</v>
+      </c>
+      <c r="Z1" s="23" t="s">
         <v>168</v>
       </c>
-      <c r="X1" s="23" t="s">
+      <c r="AA1" s="23" t="s">
         <v>169</v>
       </c>
-      <c r="Y1" s="23" t="s">
-        <v>180</v>
-      </c>
-      <c r="Z1" s="23" t="s">
+      <c r="AB1" s="23" t="s">
+        <v>179</v>
+      </c>
+      <c r="AC1" s="23" t="s">
         <v>170</v>
       </c>
-      <c r="AA1" s="23" t="s">
+      <c r="AD1" s="23" t="s">
         <v>171</v>
       </c>
-      <c r="AB1" s="23" t="s">
-        <v>181</v>
-      </c>
-      <c r="AC1" s="23" t="s">
+      <c r="AE1" s="23" t="s">
+        <v>184</v>
+      </c>
+      <c r="AF1" s="23" t="s">
         <v>172</v>
       </c>
-      <c r="AD1" s="23" t="s">
+      <c r="AG1" s="23" t="s">
         <v>173</v>
       </c>
-      <c r="AE1" s="23" t="s">
-        <v>186</v>
-      </c>
-      <c r="AF1" s="23" t="s">
+      <c r="AH1" s="23" t="s">
+        <v>182</v>
+      </c>
+      <c r="AI1" s="23" t="s">
         <v>174</v>
       </c>
-      <c r="AG1" s="23" t="s">
+      <c r="AJ1" s="23" t="s">
         <v>175</v>
       </c>
-      <c r="AH1" s="23" t="s">
-        <v>184</v>
-      </c>
-      <c r="AI1" s="23" t="s">
+      <c r="AK1" s="23" t="s">
+        <v>183</v>
+      </c>
+      <c r="AL1" s="23" t="s">
         <v>176</v>
       </c>
-      <c r="AJ1" s="23" t="s">
+      <c r="AM1" s="23" t="s">
         <v>177</v>
       </c>
-      <c r="AK1" s="23" t="s">
+      <c r="AN1" s="23" t="s">
         <v>185</v>
-      </c>
-      <c r="AL1" s="23" t="s">
-        <v>178</v>
-      </c>
-      <c r="AM1" s="23" t="s">
-        <v>179</v>
-      </c>
-      <c r="AN1" s="23" t="s">
-        <v>187</v>
       </c>
     </row>
     <row r="2" spans="1:40" x14ac:dyDescent="0.2">
@@ -8390,48 +8421,40 @@
       </c>
       <c r="C2" s="3"/>
       <c r="D2" s="10" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="E2" s="3"/>
       <c r="F2" s="3" t="s">
         <v>3</v>
       </c>
       <c r="G2" s="3" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="H2" s="3" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="I2" s="11">
-        <v>0.66666666666666663</v>
+        <v>0.5</v>
       </c>
       <c r="J2" s="11">
         <v>0.70833333333333337</v>
       </c>
       <c r="K2" s="11">
-        <v>0.4375</v>
+        <v>0.41666666666666669</v>
       </c>
       <c r="L2" s="11">
-        <v>0.52083333333333337</v>
-      </c>
-      <c r="M2" s="11">
-        <v>0.47916666666666669</v>
-      </c>
-      <c r="N2" s="11">
-        <v>0.5625</v>
-      </c>
-      <c r="O2" s="11">
-        <v>0.41666666666666669</v>
-      </c>
-      <c r="P2" s="11">
-        <v>0.54166666666666663</v>
-      </c>
-      <c r="Q2" s="11">
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="M2" s="11"/>
+      <c r="N2" s="11"/>
+      <c r="O2" s="36">
         <v>0.5</v>
       </c>
-      <c r="R2" s="11">
+      <c r="P2" s="40">
         <v>0.625</v>
       </c>
+      <c r="Q2" s="11"/>
+      <c r="R2" s="11"/>
       <c r="S2" s="11"/>
       <c r="T2" s="11"/>
       <c r="U2" s="3"/>
@@ -8443,7 +8466,7 @@
         <v>43501</v>
       </c>
       <c r="Y2" s="3" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="Z2" s="3"/>
       <c r="AA2" s="3"/>
@@ -8472,40 +8495,40 @@
         <v>136</v>
       </c>
       <c r="D3" s="10" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="E3" s="3"/>
       <c r="F3" s="3" t="s">
         <v>3</v>
       </c>
       <c r="G3" s="3" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="H3" s="3" t="s">
         <v>156</v>
       </c>
       <c r="I3" s="11">
-        <v>0.47916666666666669</v>
+        <v>0.375</v>
       </c>
       <c r="J3" s="27">
-        <v>0.60416666666666663</v>
+        <v>0.5</v>
       </c>
       <c r="K3" s="3"/>
       <c r="L3" s="3"/>
-      <c r="M3" s="11">
-        <v>0.39583333333333331</v>
-      </c>
-      <c r="N3" s="11">
-        <v>0.47916666666666669</v>
-      </c>
+      <c r="M3" s="11"/>
+      <c r="N3" s="11"/>
       <c r="O3" s="11">
-        <v>0.375</v>
+        <v>0.41666666666666669</v>
       </c>
       <c r="P3" s="11">
-        <v>0.625</v>
-      </c>
-      <c r="Q3" s="3"/>
-      <c r="R3" s="3"/>
+        <v>0.54166666666666663</v>
+      </c>
+      <c r="Q3" s="11">
+        <v>0.5</v>
+      </c>
+      <c r="R3" s="11">
+        <v>0.58333333333333337</v>
+      </c>
       <c r="S3" s="3"/>
       <c r="T3" s="3"/>
       <c r="U3" s="3"/>
@@ -8538,46 +8561,46 @@
       </c>
       <c r="C4" s="3"/>
       <c r="D4" s="10" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="E4" s="3"/>
       <c r="F4" s="3" t="s">
         <v>3</v>
       </c>
       <c r="G4" s="3" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="H4" s="3" t="s">
         <v>156</v>
       </c>
-      <c r="I4" s="11"/>
-      <c r="J4" s="11"/>
+      <c r="I4" s="11">
+        <v>0.5</v>
+      </c>
+      <c r="J4" s="38">
+        <v>0.70833333333333337</v>
+      </c>
       <c r="K4" s="11">
-        <v>0.47916666666666669</v>
+        <v>0.41666666666666669</v>
       </c>
       <c r="L4" s="11">
-        <v>0.58333333333333337</v>
-      </c>
-      <c r="M4" s="11">
-        <v>0.52083333333333337</v>
-      </c>
-      <c r="N4" s="11">
-        <v>0.60416666666666663</v>
-      </c>
-      <c r="O4" s="3"/>
-      <c r="P4" s="3"/>
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="M4" s="11"/>
+      <c r="N4" s="11"/>
+      <c r="O4" s="11">
+        <v>0.41666666666666669</v>
+      </c>
+      <c r="P4" s="11">
+        <v>0.54166666666666663</v>
+      </c>
       <c r="Q4" s="11">
         <v>0.375</v>
       </c>
       <c r="R4" s="11">
-        <v>0.54166666666666663</v>
-      </c>
-      <c r="S4" s="11">
         <v>0.41666666666666669</v>
       </c>
-      <c r="T4" s="11">
-        <v>0.58333333333333337</v>
-      </c>
+      <c r="S4" s="11"/>
+      <c r="T4" s="11"/>
       <c r="U4" s="3"/>
       <c r="V4" s="3"/>
       <c r="W4" s="3"/>
@@ -8608,42 +8631,42 @@
       </c>
       <c r="C5" s="3"/>
       <c r="D5" s="10" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="E5" s="3"/>
       <c r="F5" s="3" t="s">
         <v>3</v>
       </c>
       <c r="G5" s="3" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="H5" s="3" t="s">
         <v>156</v>
       </c>
-      <c r="I5" s="11"/>
-      <c r="J5" s="11"/>
-      <c r="K5" s="11"/>
-      <c r="L5" s="11"/>
-      <c r="M5" s="11">
+      <c r="I5" s="11">
+        <v>0.375</v>
+      </c>
+      <c r="J5" s="11">
+        <v>0.5</v>
+      </c>
+      <c r="K5" s="11">
         <v>0.41666666666666669</v>
       </c>
-      <c r="N5" s="11">
-        <v>0.58333333333333337</v>
-      </c>
-      <c r="O5" s="11"/>
-      <c r="P5" s="11"/>
-      <c r="Q5" s="11">
-        <v>0.52083333333333337</v>
-      </c>
-      <c r="R5" s="11">
-        <v>0.58333333333333337</v>
-      </c>
-      <c r="S5" s="11">
-        <v>0.375</v>
-      </c>
-      <c r="T5" s="11">
-        <v>0.70833333333333337</v>
-      </c>
+      <c r="L5" s="11">
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="M5" s="11"/>
+      <c r="N5" s="11"/>
+      <c r="O5" s="11">
+        <v>0.41666666666666669</v>
+      </c>
+      <c r="P5" s="11">
+        <v>0.54166666666666663</v>
+      </c>
+      <c r="Q5" s="11"/>
+      <c r="R5" s="11"/>
+      <c r="S5" s="11"/>
+      <c r="T5" s="11"/>
       <c r="U5" s="3"/>
       <c r="V5" s="3"/>
       <c r="W5" s="35">
@@ -8678,46 +8701,42 @@
       </c>
       <c r="C6" s="3"/>
       <c r="D6" s="10" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="E6" s="3"/>
       <c r="F6" s="3" t="s">
         <v>3</v>
       </c>
       <c r="G6" s="3" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="H6" s="3" t="s">
         <v>156</v>
       </c>
       <c r="I6" s="11">
-        <v>0.39583333333333331</v>
-      </c>
-      <c r="J6" s="11">
-        <v>0.52083333333333337</v>
+        <v>0.375</v>
+      </c>
+      <c r="J6" s="27">
+        <v>0.5</v>
       </c>
       <c r="K6" s="11"/>
       <c r="L6" s="11"/>
-      <c r="M6" s="11">
-        <v>0.45833333333333331</v>
-      </c>
-      <c r="N6" s="11">
-        <v>0.60416666666666663</v>
-      </c>
-      <c r="O6" s="11">
-        <v>0.45833333333333331</v>
-      </c>
-      <c r="P6" s="11">
-        <v>0.60416666666666663</v>
-      </c>
-      <c r="Q6" s="3"/>
-      <c r="R6" s="3"/>
-      <c r="S6" s="11">
-        <v>0.375</v>
-      </c>
-      <c r="T6" s="11">
-        <v>0.70833333333333337</v>
-      </c>
+      <c r="M6" s="11"/>
+      <c r="N6" s="11"/>
+      <c r="O6" s="36">
+        <v>0.5</v>
+      </c>
+      <c r="P6" s="40">
+        <v>0.625</v>
+      </c>
+      <c r="Q6" s="11">
+        <v>0.5</v>
+      </c>
+      <c r="R6" s="11">
+        <v>0.58333333333333337</v>
+      </c>
+      <c r="S6" s="11"/>
+      <c r="T6" s="11"/>
       <c r="U6" s="3"/>
       <c r="V6" s="3"/>
       <c r="W6" s="3"/>
@@ -8750,39 +8769,43 @@
         <v>141</v>
       </c>
       <c r="D7" s="10" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="E7" s="3"/>
       <c r="F7" s="3" t="s">
         <v>3</v>
       </c>
       <c r="G7" s="3" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="H7" s="3" t="s">
         <v>156</v>
       </c>
-      <c r="I7" s="11"/>
-      <c r="J7" s="11"/>
-      <c r="K7" s="11">
-        <v>0.39583333333333331</v>
-      </c>
-      <c r="L7" s="11">
-        <v>0.47916666666666669</v>
-      </c>
-      <c r="M7" s="11">
-        <v>0.39583333333333331</v>
-      </c>
-      <c r="N7" s="11">
-        <v>0.47916666666666669</v>
-      </c>
-      <c r="O7" s="11"/>
-      <c r="P7" s="11"/>
+      <c r="I7" s="11">
+        <v>0.5</v>
+      </c>
+      <c r="J7" s="11">
+        <v>0.70833333333333337</v>
+      </c>
+      <c r="K7" s="36">
+        <v>0.41666666666666669</v>
+      </c>
+      <c r="L7" s="40">
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="M7" s="11"/>
+      <c r="N7" s="11"/>
+      <c r="O7" s="11">
+        <v>0.41666666666666669</v>
+      </c>
+      <c r="P7" s="11">
+        <v>0.54166666666666663</v>
+      </c>
       <c r="Q7" s="11">
+        <v>0.375</v>
+      </c>
+      <c r="R7" s="11">
         <v>0.45833333333333331</v>
-      </c>
-      <c r="R7" s="11">
-        <v>0.60416666666666663</v>
       </c>
       <c r="S7" s="11"/>
       <c r="T7" s="11"/>
@@ -8816,42 +8839,42 @@
       </c>
       <c r="C8" s="3"/>
       <c r="D8" s="10" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="E8" s="3"/>
       <c r="F8" s="3" t="s">
         <v>3</v>
       </c>
       <c r="G8" s="3" t="s">
-        <v>166</v>
+        <v>188</v>
       </c>
       <c r="H8" s="3" t="s">
         <v>156</v>
       </c>
-      <c r="I8" s="11">
-        <v>0.58333333333333337</v>
-      </c>
-      <c r="J8" s="11">
+      <c r="I8" s="11"/>
+      <c r="J8" s="11"/>
+      <c r="K8" s="36">
+        <v>0.41666666666666669</v>
+      </c>
+      <c r="L8" s="40">
         <v>0.66666666666666663</v>
       </c>
-      <c r="K8" s="11"/>
-      <c r="L8" s="11"/>
       <c r="M8" s="11"/>
       <c r="N8" s="11"/>
-      <c r="O8" s="11">
-        <v>0.35416666666666669</v>
-      </c>
-      <c r="P8" s="11">
-        <v>0.47916666666666669</v>
-      </c>
-      <c r="Q8" s="3"/>
-      <c r="R8" s="3"/>
-      <c r="S8" s="11">
-        <v>0.39583333333333331</v>
-      </c>
-      <c r="T8" s="11">
-        <v>0.47916666666666669</v>
-      </c>
+      <c r="O8" s="36">
+        <v>0.5</v>
+      </c>
+      <c r="P8" s="40">
+        <v>0.625</v>
+      </c>
+      <c r="Q8" s="11">
+        <v>0.375</v>
+      </c>
+      <c r="R8" s="11">
+        <v>0.45833333333333331</v>
+      </c>
+      <c r="S8" s="11"/>
+      <c r="T8" s="11"/>
       <c r="U8" s="3"/>
       <c r="V8" s="3"/>
       <c r="W8" s="3"/>
@@ -8882,30 +8905,38 @@
       </c>
       <c r="C9" s="3"/>
       <c r="D9" s="10" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="E9" s="3"/>
       <c r="F9" s="3" t="s">
         <v>3</v>
       </c>
       <c r="G9" s="3" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="H9" s="3" t="s">
         <v>156</v>
       </c>
-      <c r="I9" s="11"/>
-      <c r="J9" s="11"/>
-      <c r="K9" s="11">
-        <v>0.39583333333333331</v>
-      </c>
-      <c r="L9" s="11">
-        <v>0.52083333333333337</v>
+      <c r="I9" s="11">
+        <v>0.375</v>
+      </c>
+      <c r="J9" s="27">
+        <v>0.5</v>
+      </c>
+      <c r="K9" s="36">
+        <v>0.41666666666666669</v>
+      </c>
+      <c r="L9" s="40">
+        <v>0.66666666666666663</v>
       </c>
       <c r="M9" s="11"/>
       <c r="N9" s="11"/>
-      <c r="O9" s="11"/>
-      <c r="P9" s="11"/>
+      <c r="O9" s="11">
+        <v>0.41666666666666669</v>
+      </c>
+      <c r="P9" s="11">
+        <v>0.54166666666666663</v>
+      </c>
       <c r="Q9" s="3"/>
       <c r="R9" s="3"/>
       <c r="S9" s="11"/>
@@ -8919,7 +8950,7 @@
         <v>43505</v>
       </c>
       <c r="Y9" s="3" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="Z9" s="3"/>
       <c r="AA9" s="3"/>
@@ -8946,39 +8977,39 @@
       </c>
       <c r="C10" s="3"/>
       <c r="D10" s="10" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="E10" s="3"/>
       <c r="F10" s="3" t="s">
         <v>3</v>
       </c>
       <c r="G10" s="3" t="s">
-        <v>167</v>
+        <v>189</v>
       </c>
       <c r="H10" s="3" t="s">
         <v>156</v>
       </c>
       <c r="I10" s="3"/>
-      <c r="J10" s="3"/>
-      <c r="K10" s="11">
-        <v>0.39583333333333331</v>
-      </c>
-      <c r="L10" s="11">
-        <v>0.5625</v>
-      </c>
-      <c r="M10" s="11">
-        <v>0.39583333333333331</v>
-      </c>
-      <c r="N10" s="11">
-        <v>0.60416666666666663</v>
-      </c>
-      <c r="O10" s="3"/>
-      <c r="P10" s="3"/>
+      <c r="J10" s="39"/>
+      <c r="K10" s="36">
+        <v>0.41666666666666669</v>
+      </c>
+      <c r="L10" s="40">
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="M10" s="11"/>
+      <c r="N10" s="11"/>
+      <c r="O10" s="36">
+        <v>0.5</v>
+      </c>
+      <c r="P10" s="40">
+        <v>0.625</v>
+      </c>
       <c r="Q10" s="11">
         <v>0.375</v>
       </c>
       <c r="R10" s="11">
-        <v>0.5</v>
+        <v>0.45833333333333331</v>
       </c>
       <c r="S10" s="3"/>
       <c r="T10" s="3"/>
@@ -9012,46 +9043,42 @@
       </c>
       <c r="C11" s="3"/>
       <c r="D11" s="10" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="E11" s="3"/>
       <c r="F11" s="3" t="s">
         <v>3</v>
       </c>
       <c r="G11" s="3" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="H11" s="3" t="s">
         <v>156</v>
       </c>
       <c r="I11" s="11">
-        <v>0.39583333333333331</v>
-      </c>
-      <c r="J11" s="11">
-        <v>0.52083333333333337</v>
-      </c>
-      <c r="K11" s="11">
+        <v>0.375</v>
+      </c>
+      <c r="J11" s="36">
         <v>0.5</v>
       </c>
-      <c r="L11" s="11">
-        <v>0.625</v>
-      </c>
+      <c r="K11" s="11"/>
+      <c r="L11" s="11"/>
       <c r="M11" s="3"/>
       <c r="N11" s="3"/>
-      <c r="O11" s="11">
-        <v>0.35416666666666669</v>
-      </c>
-      <c r="P11" s="11">
-        <v>0.5625</v>
-      </c>
-      <c r="Q11" s="3"/>
-      <c r="R11" s="3"/>
-      <c r="S11" s="11">
-        <v>0.375</v>
-      </c>
-      <c r="T11" s="11">
-        <v>0.70833333333333337</v>
-      </c>
+      <c r="O11" s="36">
+        <v>0.41666666666666669</v>
+      </c>
+      <c r="P11" s="40">
+        <v>0.54166666666666663</v>
+      </c>
+      <c r="Q11" s="11">
+        <v>0.5</v>
+      </c>
+      <c r="R11" s="11">
+        <v>0.58333333333333337</v>
+      </c>
+      <c r="S11" s="11"/>
+      <c r="T11" s="11"/>
       <c r="U11" s="3"/>
       <c r="V11" s="3"/>
       <c r="W11" s="35">
@@ -9086,50 +9113,42 @@
       </c>
       <c r="C12" s="3"/>
       <c r="D12" s="10" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="E12" s="3"/>
       <c r="F12" s="3" t="s">
         <v>3</v>
       </c>
       <c r="G12" s="3" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="H12" s="3" t="s">
         <v>156</v>
       </c>
       <c r="I12" s="11">
-        <v>0.47916666666666669</v>
-      </c>
-      <c r="J12" s="11">
-        <v>0.60416666666666663</v>
-      </c>
-      <c r="K12" s="3"/>
-      <c r="L12" s="3"/>
-      <c r="M12" s="11">
-        <v>0.39583333333333331</v>
-      </c>
-      <c r="N12" s="11">
-        <v>0.58333333333333337</v>
-      </c>
-      <c r="O12" s="11">
-        <v>0.45833333333333331</v>
-      </c>
-      <c r="P12" s="11">
-        <v>0.60416666666666663</v>
-      </c>
-      <c r="Q12" s="11">
-        <v>0.45833333333333331</v>
-      </c>
-      <c r="R12" s="11">
-        <v>0.58333333333333337</v>
-      </c>
-      <c r="S12" s="11">
         <v>0.375</v>
       </c>
-      <c r="T12" s="11">
-        <v>0.70833333333333337</v>
-      </c>
+      <c r="J12" s="27">
+        <v>0.5</v>
+      </c>
+      <c r="K12" s="36">
+        <v>0.41666666666666669</v>
+      </c>
+      <c r="L12" s="40">
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="M12" s="11"/>
+      <c r="N12" s="11"/>
+      <c r="O12" s="36">
+        <v>0.5</v>
+      </c>
+      <c r="P12" s="40">
+        <v>0.625</v>
+      </c>
+      <c r="Q12" s="11"/>
+      <c r="R12" s="11"/>
+      <c r="S12" s="11"/>
+      <c r="T12" s="11"/>
       <c r="U12" s="3"/>
       <c r="V12" s="3"/>
       <c r="W12" s="3"/>
@@ -9160,40 +9179,44 @@
       </c>
       <c r="C13" s="3"/>
       <c r="D13" s="10" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="E13" s="3"/>
       <c r="F13" s="3" t="s">
         <v>3</v>
       </c>
       <c r="G13" s="3" t="s">
-        <v>167</v>
+        <v>189</v>
       </c>
       <c r="H13" s="3" t="s">
         <v>156</v>
       </c>
-      <c r="I13" s="3"/>
-      <c r="J13" s="3"/>
-      <c r="K13" s="11">
-        <v>0.39583333333333331</v>
-      </c>
-      <c r="L13" s="11">
-        <v>0.52083333333333337</v>
-      </c>
-      <c r="M13" s="11">
-        <v>0.39583333333333331</v>
-      </c>
-      <c r="N13" s="11">
-        <v>0.60416666666666663</v>
-      </c>
-      <c r="O13" s="11">
-        <v>0.375</v>
-      </c>
-      <c r="P13" s="11">
+      <c r="I13" s="11">
         <v>0.5</v>
       </c>
-      <c r="Q13" s="3"/>
-      <c r="R13" s="3"/>
+      <c r="J13" s="11">
+        <v>0.70833333333333337</v>
+      </c>
+      <c r="K13" s="36">
+        <v>0.41666666666666669</v>
+      </c>
+      <c r="L13" s="40">
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="M13" s="11"/>
+      <c r="N13" s="11"/>
+      <c r="O13" s="36">
+        <v>0.41666666666666669</v>
+      </c>
+      <c r="P13" s="40">
+        <v>0.54166666666666663</v>
+      </c>
+      <c r="Q13" s="11">
+        <v>0.41666666666666669</v>
+      </c>
+      <c r="R13" s="11">
+        <v>0.58333333333333337</v>
+      </c>
       <c r="S13" s="3"/>
       <c r="T13" s="3"/>
       <c r="U13" s="3"/>
@@ -9226,50 +9249,38 @@
       </c>
       <c r="C14" s="3"/>
       <c r="D14" s="10" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="E14" s="3"/>
       <c r="F14" s="3" t="s">
         <v>3</v>
       </c>
       <c r="G14" s="3" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="H14" s="3" t="s">
         <v>156</v>
       </c>
-      <c r="I14" s="11">
-        <v>0.4375</v>
-      </c>
-      <c r="J14" s="11">
-        <v>0.6875</v>
-      </c>
-      <c r="K14" s="11">
-        <v>0.58333333333333337</v>
-      </c>
-      <c r="L14" s="11">
-        <v>0.6875</v>
-      </c>
+      <c r="I14" s="11"/>
+      <c r="J14" s="11"/>
+      <c r="K14" s="11"/>
+      <c r="L14" s="11"/>
       <c r="M14" s="3"/>
       <c r="N14" s="3"/>
-      <c r="O14" s="11">
-        <v>0.35416666666666669</v>
-      </c>
-      <c r="P14" s="11">
+      <c r="O14" s="36">
+        <v>0.41666666666666669</v>
+      </c>
+      <c r="P14" s="40">
+        <v>0.54166666666666663</v>
+      </c>
+      <c r="Q14" s="11">
+        <v>0.375</v>
+      </c>
+      <c r="R14" s="11">
         <v>0.45833333333333331</v>
       </c>
-      <c r="Q14" s="11">
-        <v>0.54166666666666663</v>
-      </c>
-      <c r="R14" s="11">
-        <v>0.58333333333333337</v>
-      </c>
-      <c r="S14" s="11">
-        <v>0.41666666666666669</v>
-      </c>
-      <c r="T14" s="11">
-        <v>0.58333333333333337</v>
-      </c>
+      <c r="S14" s="11"/>
+      <c r="T14" s="11"/>
       <c r="U14" s="3"/>
       <c r="V14" s="3"/>
       <c r="W14" s="3"/>
@@ -9300,42 +9311,46 @@
       </c>
       <c r="C15" s="3"/>
       <c r="D15" s="10" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="E15" s="3"/>
       <c r="F15" s="3" t="s">
         <v>3</v>
       </c>
       <c r="G15" s="3" t="s">
-        <v>165</v>
+        <v>190</v>
       </c>
       <c r="H15" s="3" t="s">
         <v>156</v>
       </c>
-      <c r="I15" s="11"/>
-      <c r="J15" s="11"/>
-      <c r="K15" s="11"/>
-      <c r="L15" s="11"/>
-      <c r="M15" s="11">
+      <c r="I15" s="11">
+        <v>0.375</v>
+      </c>
+      <c r="J15" s="27">
+        <v>0.5</v>
+      </c>
+      <c r="K15" s="36">
         <v>0.41666666666666669</v>
       </c>
-      <c r="N15" s="11">
-        <v>0.58333333333333337</v>
-      </c>
-      <c r="O15" s="11"/>
-      <c r="P15" s="11"/>
+      <c r="L15" s="40">
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="M15" s="11"/>
+      <c r="N15" s="11"/>
+      <c r="O15" s="36">
+        <v>0.41666666666666669</v>
+      </c>
+      <c r="P15" s="40">
+        <v>0.54166666666666663</v>
+      </c>
       <c r="Q15" s="11">
-        <v>0.52083333333333337</v>
+        <v>0.5</v>
       </c>
       <c r="R15" s="11">
         <v>0.58333333333333337</v>
       </c>
-      <c r="S15" s="11">
-        <v>0.45833333333333331</v>
-      </c>
-      <c r="T15" s="11">
-        <v>0.60416666666666663</v>
-      </c>
+      <c r="S15" s="11"/>
+      <c r="T15" s="11"/>
       <c r="U15" s="3"/>
       <c r="V15" s="3"/>
       <c r="W15" s="3"/>
@@ -9362,11 +9377,11 @@
         <v>48</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="C16" s="3"/>
       <c r="D16" s="10" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="E16" s="3"/>
       <c r="F16" s="3" t="s">
@@ -9374,36 +9389,36 @@
       </c>
       <c r="G16" s="3"/>
       <c r="H16" s="3" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="I16" s="11">
-        <v>0.39583333333333331</v>
+        <v>0.5</v>
       </c>
       <c r="J16" s="11">
-        <v>0.52083333333333337</v>
-      </c>
-      <c r="K16" s="11"/>
-      <c r="L16" s="11"/>
-      <c r="M16" s="11">
+        <v>0.70833333333333337</v>
+      </c>
+      <c r="K16" s="36">
+        <v>0.41666666666666669</v>
+      </c>
+      <c r="L16" s="40">
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="M16" s="11"/>
+      <c r="N16" s="11"/>
+      <c r="O16" s="11">
+        <v>0.5</v>
+      </c>
+      <c r="P16" s="11">
+        <v>0.625</v>
+      </c>
+      <c r="Q16" s="11">
+        <v>0.375</v>
+      </c>
+      <c r="R16" s="11">
         <v>0.45833333333333331</v>
       </c>
-      <c r="N16" s="11">
-        <v>0.60416666666666663</v>
-      </c>
-      <c r="O16" s="11">
-        <v>0.45833333333333331</v>
-      </c>
-      <c r="P16" s="11">
-        <v>0.60416666666666663</v>
-      </c>
-      <c r="Q16" s="3"/>
-      <c r="R16" s="3"/>
-      <c r="S16" s="11">
-        <v>0.39583333333333331</v>
-      </c>
-      <c r="T16" s="11">
-        <v>0.47916666666666669</v>
-      </c>
+      <c r="S16" s="11"/>
+      <c r="T16" s="11"/>
       <c r="U16" s="3"/>
       <c r="V16" s="3"/>
       <c r="W16" s="3"/>
@@ -9430,11 +9445,11 @@
         <v>48</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="C17" s="3"/>
       <c r="D17" s="10" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="E17" s="3"/>
       <c r="F17" s="3" t="s">
@@ -9446,32 +9461,28 @@
       </c>
       <c r="I17" s="11"/>
       <c r="J17" s="11"/>
-      <c r="K17" s="11">
-        <v>0.39583333333333331</v>
-      </c>
-      <c r="L17" s="11">
-        <v>0.47916666666666669</v>
-      </c>
-      <c r="M17" s="11">
-        <v>0.39583333333333331</v>
-      </c>
-      <c r="N17" s="11">
-        <v>0.47916666666666669</v>
-      </c>
-      <c r="O17" s="11"/>
-      <c r="P17" s="11"/>
+      <c r="K17" s="36">
+        <v>0.41666666666666669</v>
+      </c>
+      <c r="L17" s="40">
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="M17" s="11"/>
+      <c r="N17" s="11"/>
+      <c r="O17" s="36">
+        <v>0.41666666666666669</v>
+      </c>
+      <c r="P17" s="40">
+        <v>0.54166666666666663</v>
+      </c>
       <c r="Q17" s="11">
-        <v>0.45833333333333331</v>
+        <v>0.5</v>
       </c>
       <c r="R17" s="11">
-        <v>0.60416666666666663</v>
-      </c>
-      <c r="S17" s="11">
-        <v>0.375</v>
-      </c>
-      <c r="T17" s="11">
-        <v>0.70833333333333337</v>
-      </c>
+        <v>0.58333333333333337</v>
+      </c>
+      <c r="S17" s="11"/>
+      <c r="T17" s="11"/>
       <c r="U17" s="3"/>
       <c r="V17" s="3"/>
       <c r="W17" s="3"/>
@@ -9498,41 +9509,37 @@
         <v>48</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="C18" s="3"/>
       <c r="D18" s="10" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="E18" s="3"/>
       <c r="F18" s="3" t="s">
         <v>3</v>
       </c>
       <c r="G18" s="3" t="s">
-        <v>13</v>
+        <v>164</v>
       </c>
       <c r="H18" s="3" t="s">
         <v>156</v>
       </c>
-      <c r="I18" s="11">
-        <v>0.58333333333333337</v>
-      </c>
-      <c r="J18" s="11">
-        <v>0.66666666666666663</v>
+      <c r="I18" s="36">
+        <v>0.375</v>
+      </c>
+      <c r="J18" s="37">
+        <v>0.5</v>
       </c>
       <c r="K18" s="11"/>
       <c r="L18" s="11"/>
-      <c r="M18" s="11">
-        <v>0.375</v>
-      </c>
-      <c r="N18" s="11">
-        <v>0.70833333333333337</v>
-      </c>
-      <c r="O18" s="11">
-        <v>0.35416666666666669</v>
-      </c>
-      <c r="P18" s="11">
-        <v>0.47916666666666669</v>
+      <c r="M18" s="11"/>
+      <c r="N18" s="11"/>
+      <c r="O18" s="36">
+        <v>0.41666666666666669</v>
+      </c>
+      <c r="P18" s="40">
+        <v>0.54166666666666663</v>
       </c>
       <c r="Q18" s="3"/>
       <c r="R18" s="3"/>
@@ -9568,7 +9575,7 @@
       </c>
       <c r="C19" s="3"/>
       <c r="D19" s="10" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="E19" s="3"/>
       <c r="F19" s="3" t="s">
@@ -9581,37 +9588,25 @@
         <v>156</v>
       </c>
       <c r="I19" s="11">
+        <v>0.5</v>
+      </c>
+      <c r="J19" s="11">
+        <v>0.70833333333333337</v>
+      </c>
+      <c r="K19" s="36">
         <v>0.41666666666666669</v>
       </c>
-      <c r="J19" s="11">
-        <v>0.5</v>
-      </c>
-      <c r="K19" s="11">
-        <v>0.45833333333333331</v>
-      </c>
-      <c r="L19" s="11">
-        <v>0.54166666666666663</v>
+      <c r="L19" s="40">
+        <v>0.66666666666666663</v>
       </c>
       <c r="M19" s="3"/>
       <c r="N19" s="3"/>
-      <c r="O19" s="11">
-        <v>0.375</v>
-      </c>
-      <c r="P19" s="11">
-        <v>0.54166666666666663</v>
-      </c>
-      <c r="Q19" s="11">
-        <v>0.41666666666666669</v>
-      </c>
-      <c r="R19" s="11">
-        <v>0.58333333333333337</v>
-      </c>
-      <c r="S19" s="11">
-        <v>0.375</v>
-      </c>
-      <c r="T19" s="11">
-        <v>0.70833333333333337</v>
-      </c>
+      <c r="O19" s="11"/>
+      <c r="P19" s="11"/>
+      <c r="Q19" s="11"/>
+      <c r="R19" s="11"/>
+      <c r="S19" s="11"/>
+      <c r="T19" s="11"/>
       <c r="U19" s="3"/>
       <c r="V19" s="3"/>
       <c r="W19" s="3"/>
@@ -10643,7 +10638,7 @@
     </row>
   </sheetData>
   <dataValidations count="5">
-    <dataValidation type="time" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="S2:V43 I2:J2 I3 K2:N43 Q2:R24 Q27:R27 P25:P26 J29:J30 I4:J28 I31:J43 O19:P21 P22:P23 O24:P24 O27:P43 P2:P18 R25:R26 R28:R43" xr:uid="{00000000-0002-0000-0400-000000000000}">
+    <dataValidation type="time" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="S2:V43 I4:J4 I3 I11:I12 O7:R7 Q27:R27 P25:P26 J29:J30 R28:R43 I31:J43 O19:P21 P22:P23 O24:P24 O27:P43 K18:L18 R25:R26 I13:J14 I5:I6 I7:J8 I9 I10:J10 I19:J28 I2:L2 I15 I16:J17 M2:N43 K14:L14 Q17:R24 J5 K20:L43 O9:P9 O3:P5 P16:R16 Q2:R6 Q8:R15 K3:L6 K11:L11" xr:uid="{00000000-0002-0000-0400-000000000000}">
       <formula1>0.375</formula1>
       <formula2>0.708333333333333</formula2>
     </dataValidation>
@@ -10656,7 +10651,7 @@
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A2:A43" xr:uid="{00000000-0002-0000-0400-000003000000}">
       <formula1>"Facilitator,Guest Speaker"</formula1>
     </dataValidation>
-    <dataValidation type="time" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="O25:O26 Q1 O2:O18 I29:I30 O22:O23 Q25:Q26 Q28:Q1048576" xr:uid="{00000000-0002-0000-0400-000004000000}">
+    <dataValidation type="time" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="O25:O26 Q1 Q28:Q1048576 I29:I30 O22:O23 Q25:Q26 O16" xr:uid="{00000000-0002-0000-0400-000004000000}">
       <formula1>0.354166666666667</formula1>
       <formula2>0.708333333333333</formula2>
     </dataValidation>
@@ -10681,10 +10676,10 @@
   <dimension ref="A1:Y1207"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScale="98" zoomScaleNormal="98" zoomScalePageLayoutView="98" workbookViewId="0">
-      <pane xSplit="2" ySplit="7" topLeftCell="C8" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="7" topLeftCell="C10" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="C8" sqref="C8"/>
+      <selection pane="bottomRight" activeCell="G20" sqref="G20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="0" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -10706,60 +10701,60 @@
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.2">
       <c r="B2"/>
-      <c r="C2" s="42" t="s">
+      <c r="C2" s="47" t="s">
         <v>82</v>
       </c>
-      <c r="D2" s="42"/>
-      <c r="E2" s="42"/>
-      <c r="F2" s="42"/>
-      <c r="G2" s="42"/>
-      <c r="H2" s="42"/>
-      <c r="I2" s="42"/>
-      <c r="J2" s="42"/>
-      <c r="K2" s="42"/>
-      <c r="N2" s="43">
+      <c r="D2" s="47"/>
+      <c r="E2" s="47"/>
+      <c r="F2" s="47"/>
+      <c r="G2" s="47"/>
+      <c r="H2" s="47"/>
+      <c r="I2" s="47"/>
+      <c r="J2" s="47"/>
+      <c r="K2" s="47"/>
+      <c r="N2" s="48">
         <f ca="1">TODAY()</f>
-        <v>43746</v>
+        <v>43748</v>
       </c>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.2">
       <c r="B3"/>
-      <c r="C3" s="42"/>
-      <c r="D3" s="42"/>
-      <c r="E3" s="42"/>
-      <c r="F3" s="42"/>
-      <c r="G3" s="42"/>
-      <c r="H3" s="42"/>
-      <c r="I3" s="42"/>
-      <c r="J3" s="42"/>
-      <c r="K3" s="42"/>
-      <c r="N3" s="44"/>
+      <c r="C3" s="47"/>
+      <c r="D3" s="47"/>
+      <c r="E3" s="47"/>
+      <c r="F3" s="47"/>
+      <c r="G3" s="47"/>
+      <c r="H3" s="47"/>
+      <c r="I3" s="47"/>
+      <c r="J3" s="47"/>
+      <c r="K3" s="47"/>
+      <c r="N3" s="49"/>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.2">
       <c r="B4"/>
-      <c r="C4" s="42"/>
-      <c r="D4" s="42"/>
-      <c r="E4" s="42"/>
-      <c r="F4" s="42"/>
-      <c r="G4" s="42"/>
-      <c r="H4" s="42"/>
-      <c r="I4" s="42"/>
-      <c r="J4" s="42"/>
-      <c r="K4" s="42"/>
-      <c r="N4" s="44"/>
+      <c r="C4" s="47"/>
+      <c r="D4" s="47"/>
+      <c r="E4" s="47"/>
+      <c r="F4" s="47"/>
+      <c r="G4" s="47"/>
+      <c r="H4" s="47"/>
+      <c r="I4" s="47"/>
+      <c r="J4" s="47"/>
+      <c r="K4" s="47"/>
+      <c r="N4" s="49"/>
     </row>
     <row r="5" spans="1:15" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B5"/>
-      <c r="C5" s="42"/>
-      <c r="D5" s="42"/>
-      <c r="E5" s="42"/>
-      <c r="F5" s="42"/>
-      <c r="G5" s="42"/>
-      <c r="H5" s="42"/>
-      <c r="I5" s="42"/>
-      <c r="J5" s="42"/>
-      <c r="K5" s="42"/>
-      <c r="N5" s="45"/>
+      <c r="C5" s="47"/>
+      <c r="D5" s="47"/>
+      <c r="E5" s="47"/>
+      <c r="F5" s="47"/>
+      <c r="G5" s="47"/>
+      <c r="H5" s="47"/>
+      <c r="I5" s="47"/>
+      <c r="J5" s="47"/>
+      <c r="K5" s="47"/>
+      <c r="N5" s="50"/>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.2">
       <c r="B6"/>
@@ -11174,7 +11169,7 @@
         <v>61</v>
       </c>
       <c r="G15" s="6" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="H15" s="6">
         <v>25</v>
@@ -11324,7 +11319,7 @@
         <v>61</v>
       </c>
       <c r="G18" s="6" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="H18" s="6">
         <v>20</v>

</xml_diff>